<commit_message>
The report on lab work 2 has been fully written. The research on lab work 2 has been corrected.
</commit_message>
<xml_diff>
--- a/Лаба 2/Результаты/Полученные результаты/Нормальное распределение/Файлы таблиц резальтатов/Калмогоров_result.xlsx
+++ b/Лаба 2/Результаты/Полученные результаты/Нормальное распределение/Файлы таблиц резальтатов/Калмогоров_result.xlsx
@@ -1,43 +1,113 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="600" yWindow="615" windowWidth="12135" windowHeight="10170"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Калмогоров" sheetId="1" r:id="rId1"/>
+    <sheet name="Крамера-Мизиса-Смирнова" sheetId="2" r:id="rId2"/>
+    <sheet name="Андерсон-Дарлинг" sheetId="3" r:id="rId3"/>
+    <sheet name="Хи-квадрат" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
+  <si>
+    <t>a(1)</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Критерий Хи-квадрат</t>
+  </si>
+  <si>
+    <t>Критерий Калмогорова</t>
+  </si>
+  <si>
+    <t>Критерий Крамера-Мизиса-Смирнова</t>
+  </si>
+  <si>
+    <t>Критерий Андерсона-Дарлинга</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="7">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -46,93 +116,82 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -420,70 +479,477 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>0.4642</v>
+      </c>
+      <c r="D2">
+        <v>0.90149999999999997</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>0.58879999999999999</v>
+      </c>
+      <c r="D3">
+        <v>0.58389999999999997</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="J5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="J6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>500</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="J7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="J8" s="6">
+        <v>4</v>
+      </c>
+      <c r="K8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>0.4642</v>
+      </c>
+      <c r="L8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.90149999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="J9" s="6">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>0.58879999999999999</v>
+      </c>
+      <c r="L9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.58389999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="J5:L5"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="J5" sqref="J5:L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>a(1)</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:12">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
         <v>4</v>
       </c>
-      <c r="B2" t="n">
-        <v>500</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.4642</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.9015</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="D2">
+        <v>0.78190000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
         <v>5</v>
       </c>
-      <c r="B3" t="n">
-        <v>500</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.5888</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.5839</v>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>3.95E-2</v>
+      </c>
+      <c r="D3">
+        <v>0.68269999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="J5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="J6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>500</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="J7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="J8" s="6">
+        <v>4</v>
+      </c>
+      <c r="K8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="L8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.78190000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="J9" s="6">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>3.95E-2</v>
+      </c>
+      <c r="L9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.68269999999999997</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <mergeCells count="2">
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="K6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>0.2278</v>
+      </c>
+      <c r="D2">
+        <v>0.81410000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>0.26140000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.71809999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="J5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="J6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>500</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="J7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="J8" s="6">
+        <v>4</v>
+      </c>
+      <c r="K8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>0.2278</v>
+      </c>
+      <c r="L8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.81410000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="J9" s="6">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>0.26140000000000002</v>
+      </c>
+      <c r="L9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.71809999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75">
+      <c r="G16" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="K6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>500</v>
+      </c>
+      <c r="C2">
+        <v>2.8035999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.59119999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>5.0708000000000002</v>
+      </c>
+      <c r="D3">
+        <v>0.28010000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75">
+      <c r="J5" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="J6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="4">
+        <v>500</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="J7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="J8" s="6">
+        <v>4</v>
+      </c>
+      <c r="K8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>2.8035999999999999</v>
+      </c>
+      <c r="L8" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J8,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.59119999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="J9" s="6">
+        <v>5</v>
+      </c>
+      <c r="K9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,2)</f>
+        <v>5.0708000000000002</v>
+      </c>
+      <c r="L9" s="6">
+        <f ca="1">OFFSET($A$2,MATCH($J9,$A$2:$A$19,0)+MATCH(K$6,$B$2:$B$4,0)-2,3)</f>
+        <v>0.28010000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="K6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>